<commit_message>
finish port review, needs cleaning
</commit_message>
<xml_diff>
--- a/portfolio_weight_calculator.xlsx
+++ b/portfolio_weight_calculator.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MilesChild/Desktop/Student Value Fund/pm/svf_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC7861BE-FE3D-7F48-AEC9-ED19768B11F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6149AB59-CD77-2D4B-A3A4-0F2387AF95B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F6784512-DCF3-9845-8481-834CE950B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculator" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -446,19 +447,10 @@
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -477,10 +469,10 @@
     <xf numFmtId="10" fontId="5" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -510,7 +502,7 @@
     <xf numFmtId="10" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="5" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -542,6 +534,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="3" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -972,7 +973,7 @@
   <dimension ref="B1:L52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -994,816 +995,816 @@
     </row>
     <row r="3" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="H4" s="2" t="s">
+      <c r="B4" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="35"/>
+      <c r="H4" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="153" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="25"/>
-      <c r="H7" s="27">
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="22"/>
+      <c r="H7" s="24">
         <v>0.75</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="28">
         <f>1-SUM(I8:I15)</f>
         <v>0.41321801319687923</v>
       </c>
-      <c r="J7" s="30"/>
+      <c r="J7" s="27"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="25"/>
-      <c r="H8" s="28">
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="22"/>
+      <c r="H8" s="25">
         <v>9.0800000000000006E-2</v>
       </c>
-      <c r="I8" s="32">
+      <c r="I8" s="29">
         <v>9.0800000000000006E-2</v>
       </c>
-      <c r="K8" s="30"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="25"/>
-      <c r="H9" s="28">
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="22"/>
+      <c r="H9" s="25">
         <v>0.11</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="29">
         <v>0.11</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="6">
         <v>0.1</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="10">
         <v>0.4</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="6">
         <v>0.5</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="7">
         <v>0.25</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="26">
         <f>IFERROR((C10+(D10-((1-D10)/(E10/F10))))/4, )</f>
         <v>5.000000000000001E-2</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="30">
         <f>H10/SUM($H$7:$H$52)</f>
         <v>3.2289546339760181E-2</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="6">
         <v>0.05</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="10">
         <v>0.25</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="6">
         <v>3</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="7">
         <v>0.65</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11" s="26">
         <f t="shared" ref="H11:H52" si="0">IFERROR((C11+(D11-((1-D11)/(E11/F11))))/4, )</f>
         <v>3.4375000000000003E-2</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="30">
         <f t="shared" ref="I11:I52" si="1">H11/SUM($H$7:$H$52)</f>
         <v>2.2199063108585118E-2</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="6">
         <v>0.2</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="10">
         <v>0.5</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="6">
         <v>0.3</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="7">
         <v>0.25</v>
       </c>
-      <c r="H12" s="29">
+      <c r="H12" s="26">
         <f t="shared" si="0"/>
         <v>7.0833333333333331E-2</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="30">
         <f t="shared" si="1"/>
         <v>4.574352398132691E-2</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="6">
         <v>0.1</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="10">
         <v>0.4</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="6">
         <v>0.5</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="7">
         <v>0.25</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" s="26">
         <f t="shared" si="0"/>
         <v>5.000000000000001E-2</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="30">
         <f t="shared" si="1"/>
         <v>3.2289546339760181E-2</v>
       </c>
-      <c r="K13" s="30"/>
+      <c r="K13" s="27"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="10">
         <v>0.7</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="6">
         <v>1.599</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="7">
         <v>0.29299999999999998</v>
       </c>
-      <c r="H14" s="29">
+      <c r="H14" s="26">
         <f t="shared" si="0"/>
         <v>0.17875703564727952</v>
       </c>
-      <c r="I14" s="33">
+      <c r="I14" s="30">
         <f t="shared" si="1"/>
         <v>0.11543967172181986</v>
       </c>
-      <c r="K14" s="30"/>
+      <c r="K14" s="27"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="6">
         <v>0.34</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="10">
         <v>0.6</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="6">
         <v>2.35</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="7">
         <v>0.5</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H15" s="26">
         <f t="shared" si="0"/>
         <v>0.21372340425531916</v>
       </c>
-      <c r="I15" s="33">
+      <c r="I15" s="30">
         <f t="shared" si="1"/>
         <v>0.13802063531186848</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="7"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="10"/>
-      <c r="H16" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="33">
+      <c r="B16" s="4"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="H16" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="7"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="10"/>
-      <c r="H17" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="33">
+      <c r="B17" s="4"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
+      <c r="H17" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="7"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="10"/>
-      <c r="H18" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="33">
+      <c r="B18" s="4"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
+      <c r="H18" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="7"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="10"/>
-      <c r="H19" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="33">
+      <c r="B19" s="4"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7"/>
+      <c r="H19" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="7"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="10"/>
-      <c r="H20" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="33">
+      <c r="B20" s="4"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="H20" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="7"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10"/>
-      <c r="H21" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="33">
+      <c r="B21" s="4"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="H21" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="7"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="10"/>
-      <c r="H22" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="33">
+      <c r="B22" s="4"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
+      <c r="H22" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="7"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="10"/>
-      <c r="H23" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="33">
+      <c r="B23" s="4"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
+      <c r="H23" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="7"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="10"/>
-      <c r="H24" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="33">
+      <c r="B24" s="4"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="H24" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="7"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="10"/>
-      <c r="H25" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="33">
+      <c r="B25" s="4"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="H25" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="7"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="10"/>
-      <c r="H26" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="33">
+      <c r="B26" s="4"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="H26" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="7"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="10"/>
-      <c r="H27" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="33">
+      <c r="B27" s="4"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="7"/>
+      <c r="H27" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="7"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="10"/>
-      <c r="H28" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="33">
+      <c r="B28" s="4"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
+      <c r="H28" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="7"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="10"/>
-      <c r="H29" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I29" s="33">
+      <c r="B29" s="4"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+      <c r="H29" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B30" s="7"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="10"/>
-      <c r="H30" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="33">
+      <c r="B30" s="4"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
+      <c r="H30" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="7"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="10"/>
-      <c r="H31" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="33">
+      <c r="B31" s="4"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
+      <c r="H31" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="7"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="10"/>
-      <c r="H32" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="33">
+      <c r="B32" s="4"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="7"/>
+      <c r="H32" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="7"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="10"/>
-      <c r="H33" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="33">
+      <c r="B33" s="4"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+      <c r="H33" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="7"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="10"/>
-      <c r="H34" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I34" s="33">
+      <c r="B34" s="4"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="7"/>
+      <c r="H34" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B35" s="7"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="10"/>
-      <c r="H35" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="33">
+      <c r="B35" s="4"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="7"/>
+      <c r="H35" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="7"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="10"/>
-      <c r="H36" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I36" s="33">
+      <c r="B36" s="4"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="7"/>
+      <c r="H36" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B37" s="7"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="10"/>
-      <c r="H37" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I37" s="33">
+      <c r="B37" s="4"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="7"/>
+      <c r="H37" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I37" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="7"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="10"/>
-      <c r="H38" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I38" s="33">
+      <c r="B38" s="4"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="7"/>
+      <c r="H38" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B39" s="7"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="10"/>
-      <c r="H39" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I39" s="33">
+      <c r="B39" s="4"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="7"/>
+      <c r="H39" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B40" s="7"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="10"/>
-      <c r="H40" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I40" s="33">
+      <c r="B40" s="4"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="7"/>
+      <c r="H40" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B41" s="7"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="10"/>
-      <c r="H41" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I41" s="33">
+      <c r="B41" s="4"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="7"/>
+      <c r="H41" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I41" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B42" s="7"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="10"/>
-      <c r="H42" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I42" s="33">
+      <c r="B42" s="4"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="7"/>
+      <c r="H42" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B43" s="7"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="10"/>
-      <c r="H43" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I43" s="33">
+      <c r="B43" s="4"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="7"/>
+      <c r="H43" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B44" s="7"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="10"/>
-      <c r="H44" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I44" s="33">
+      <c r="B44" s="4"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="7"/>
+      <c r="H44" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I44" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B45" s="7"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="10"/>
-      <c r="H45" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I45" s="33">
+      <c r="B45" s="4"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="7"/>
+      <c r="H45" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I45" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B46" s="7"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="10"/>
-      <c r="H46" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I46" s="33">
+      <c r="B46" s="4"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="7"/>
+      <c r="H46" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I46" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B47" s="7"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="10"/>
-      <c r="H47" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I47" s="33">
+      <c r="B47" s="4"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="7"/>
+      <c r="H47" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I47" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B48" s="7"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="10"/>
-      <c r="H48" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I48" s="33">
+      <c r="B48" s="4"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="7"/>
+      <c r="H48" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B49" s="7"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="10"/>
-      <c r="H49" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I49" s="33">
+      <c r="B49" s="4"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="7"/>
+      <c r="H49" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I49" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B50" s="7"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="10"/>
-      <c r="H50" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I50" s="33">
+      <c r="B50" s="4"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="7"/>
+      <c r="H50" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I50" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B51" s="7"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="10"/>
-      <c r="H51" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I51" s="33">
+      <c r="B51" s="4"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="7"/>
+      <c r="H51" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I51" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="8"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="12"/>
-      <c r="H52" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I52" s="34">
+      <c r="B52" s="5"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="9"/>
+      <c r="H52" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I52" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1816,4 +1817,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D660E4FC-B373-0841-9EFD-D2C67613775F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>